<commit_message>
added tags for demo
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/salesperson_test_data.xlsx
+++ b/TestData/Web_POS/Billing/salesperson_test_data.xlsx
@@ -1,216 +1,197 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Web_POS\Billing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="48">
-  <si>
-    <t xml:space="preserve">TC_Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serial_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password_pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closing_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opening_balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assortment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buy_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manual_discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discount_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carry_bag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price_Override</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salesperson_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_salesperson_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t>TC_Id</t>
+  </si>
+  <si>
+    <t>serial_key</t>
+  </si>
+  <si>
+    <t>username_admin</t>
+  </si>
+  <si>
+    <t>password_admin</t>
+  </si>
+  <si>
+    <t>username_pos</t>
+  </si>
+  <si>
+    <t>password_pos</t>
+  </si>
+  <si>
+    <t>closing_balance</t>
+  </si>
+  <si>
+    <t>opening_balance</t>
+  </si>
+  <si>
+    <t>store_name</t>
+  </si>
+  <si>
+    <t>assortment</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>buy_items</t>
+  </si>
+  <si>
+    <t>get_items</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>manual_discount</t>
+  </si>
+  <si>
+    <t>discount_value</t>
+  </si>
+  <si>
+    <t>carry_bag</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Price_Override</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>salesperson_name</t>
+  </si>
+  <si>
+    <t>new_salesperson_name</t>
+  </si>
+  <si>
+    <t>TC_1</t>
   </si>
   <si>
     <t xml:space="preserve">3072006242zn </t>
   </si>
   <si>
-    <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
+    <t>zwshashank.agrawal@teampureplay.com</t>
   </si>
   <si>
     <t xml:space="preserve">AdityaWagh </t>
   </si>
   <si>
-    <t xml:space="preserve">Index9QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8906118412556 : 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dummy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saloni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_5</t>
+    <t>Index9QA</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>8906118412556 : 2</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>TC_2</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t>Saloni</t>
+  </si>
+  <si>
+    <t>TC_5</t>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="10"/>
+        <scheme val="none"/>
       </rPr>
-      <t xml:space="preserve">8906118412556</t>
+      <t>8906118412556</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
         <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <scheme val="none"/>
       </rPr>
       <t xml:space="preserve"> : 1, HJ001111 : 1</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">TC_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarth jha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_10</t>
+    <t>TC_6</t>
+  </si>
+  <si>
+    <t>TC_7</t>
+  </si>
+  <si>
+    <t>TC_8</t>
+  </si>
+  <si>
+    <t>Sarth jha</t>
+  </si>
+  <si>
+    <t>TC_9</t>
+  </si>
+  <si>
+    <t>TC_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -223,7 +204,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -256,115 +236,349 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AB11"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="14" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="11.52"/>
+    <col min="1" max="1" width="11.52"/>
+    <col min="2" max="2" width="14.88" customWidth="1"/>
+    <col min="3" max="3" width="34.91" customWidth="1"/>
+    <col min="4" max="4" width="16.17" customWidth="1"/>
+    <col min="5" max="5" width="14.35" customWidth="1"/>
+    <col min="6" max="6" width="14.01" customWidth="1"/>
+    <col min="7" max="7" width="14.43" customWidth="1"/>
+    <col min="8" max="8" width="15.68" customWidth="1"/>
+    <col min="9" max="12" width="11.52"/>
+    <col min="13" max="13" width="29.24" customWidth="1"/>
+    <col min="14" max="22" width="11.52"/>
+    <col min="23" max="23" width="14.4" customWidth="1"/>
+    <col min="24" max="25" width="11.52"/>
+    <col min="26" max="26" width="22.09" customWidth="1"/>
+    <col min="27" max="1025" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +662,7 @@
       </c>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -458,19 +672,19 @@
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>123456</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="1">
         <v>1000</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>600</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -528,7 +742,7 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -538,19 +752,19 @@
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>123456</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="F3" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G3" s="1">
         <v>1000</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>600</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -607,7 +821,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -617,19 +831,19 @@
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>123456</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G4" s="1" t="n">
+      <c r="F4" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G4" s="1">
         <v>1000</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>600</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -685,7 +899,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -695,19 +909,19 @@
       <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="1">
         <v>123456</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G5" s="1" t="n">
+      <c r="F5" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G5" s="1">
         <v>1000</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>600</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -763,7 +977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" ht="22.2" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -773,19 +987,19 @@
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="1">
         <v>123456</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G6" s="1" t="n">
+      <c r="F6" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G6" s="1">
         <v>1000</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>600</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -841,7 +1055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -851,19 +1065,19 @@
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>123456</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="1">
         <v>1000</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -919,7 +1133,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -929,19 +1143,19 @@
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="1">
         <v>123456</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G8" s="1" t="n">
+      <c r="F8" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G8" s="1">
         <v>1000</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -997,7 +1211,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1007,19 +1221,19 @@
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="1">
         <v>123456</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G9" s="1" t="n">
+      <c r="F9" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G9" s="1">
         <v>1000</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -1074,11 +1288,11 @@
       <c r="Z9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="0" t="s">
+      <c r="AA9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1088,19 +1302,19 @@
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="1">
         <v>123456</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G10" s="1" t="n">
+      <c r="F10" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G10" s="1">
         <v>1000</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -1155,11 +1369,11 @@
       <c r="Z10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA10" s="0" t="s">
+      <c r="AA10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1169,19 +1383,19 @@
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="1">
         <v>123456</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="1" t="n">
+      <c r="F11" s="1">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="1">
         <v>1000</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="1">
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1238,10 +1452,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.7875" right="0.7875" top="1.052778" bottom="1.052778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>